<commit_message>
Ajout de la présentation de gestion
</commit_message>
<xml_diff>
--- a/0100_Research/0120_Prototypes/0122_LiDarLitev4/0_ErrorCharacteristic/Error Characteristics.xlsx
+++ b/0100_Research/0120_Prototypes/0122_LiDarLitev4/0_ErrorCharacteristic/Error Characteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e675ddd269f32ab/Documents/3e/PGA/git/LoRaSnow/0100_Research/0120_Prototypes/0122_LiDarLitev4/0_ErrorCharacteristic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_AD4D9D64A577C15A4A5418AA809858665BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C212623-3ADD-4C42-A0B0-7F36EC332646}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_AD4D9D64A577C15A4A5418AA809858665BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37D7BE86-92C3-4D41-9282-5A95FC15CC02}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="25°C" sheetId="1" r:id="rId1"/>
@@ -1465,7 +1465,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Error</a:t>
+              <a:t>Error </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -5144,8 +5144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>